<commit_message>
added new content to data
</commit_message>
<xml_diff>
--- a/PS-250/Radioactivity_Lab/LabData.xlsx
+++ b/PS-250/Radioactivity_Lab/LabData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevStark\Github\Fall_2018_Homework\PS-250\Radioactivity_Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stark/StarkDev/Fall_2018_Homework/PS-250/Radioactivity_Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9210491D-24C4-468E-A3CD-3794079EB05F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9638356-EE29-904E-A875-7B6E2FCA583D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20130" windowHeight="13890" xr2:uid="{1A1AC8B1-93FF-4B55-B881-409B33EC84FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15420" windowHeight="18000" xr2:uid="{1A1AC8B1-93FF-4B55-B881-409B33EC84FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$301</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Run #1 No Pb or Al</t>
   </si>
   <si>
     <t xml:space="preserve"> Pb Plates cm</t>
-  </si>
-  <si>
-    <t>Al plates 1.3x10-6</t>
   </si>
   <si>
     <t>Run #2 - No plates</t>
@@ -80,12 +77,36 @@
   <si>
     <t>Run #14 - Al 30</t>
   </si>
+  <si>
+    <t>Absorbtion Coeficient Pb</t>
+  </si>
+  <si>
+    <t>Absorbtion Coeffiecient Al</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al plates </t>
+  </si>
+  <si>
+    <t>Average Values for Co-60</t>
+  </si>
+  <si>
+    <t>Average Values for Sr-90</t>
+  </si>
+  <si>
+    <t>Blocking Effectiveness % Pb</t>
+  </si>
+  <si>
+    <t>Blocking Effectiveness % Al</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,12 +172,748 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ln(N)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs X for Co-60</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.6501472588235693</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9113618185921677</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5686309229805193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4260000479346377</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2191456736714752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.820060757608986</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6369007278824137</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6136-1747-8EC2-39C5BACCA2EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1062615392"/>
+        <c:axId val="1058517456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1062615392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1058517456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1058517456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1062615392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ln(N)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs X for Sr-90</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4999999999999996E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2500000000000004E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8999999999999999E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.2105999795246527</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2038836475592154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1202964439509504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0014129279611508</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9089858877837438</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8579302294834585</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6DA2-3A4E-B52B-61D945C2EC21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1061994784"/>
+        <c:axId val="1061778688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1061994784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1061778688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1061778688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1061994784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -194,7 +951,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{98365BB7-E504-43B2-AF53-D63ADD89C43C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Run #1 No Pb or Al</cx:v>
             </cx:txData>
           </cx:tx>
@@ -263,6 +1020,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -767,6 +1604,1038 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -775,15 +2644,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1409700</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1704975</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:colOff>1933575</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -820,8 +2689,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2914650" y="4167187"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="3352800" y="3662362"/>
+              <a:ext cx="5184775" cy="2552700"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -849,6 +2718,78 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{011F9303-A659-A14D-8AD9-A8BCC4F30184}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3668B326-6E91-F048-BE2D-192DB75A9C1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1151,27 +3092,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908E722D-64B1-4FB9-A7CE-2ED9FD62516E}">
-  <dimension ref="A1:I301"/>
+  <dimension ref="A1:K301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1179,28 +3122,34 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0.15</v>
       </c>
@@ -1228,8 +3177,16 @@
       <c r="I2" s="1">
         <v>157</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="1">
+        <f>C6</f>
+        <v>5.6501472588235693</v>
+      </c>
+      <c r="K2" s="1">
+        <f>C12</f>
+        <v>6.2105999795246527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -1257,8 +3214,16 @@
       <c r="I3" s="1">
         <v>168</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="1">
+        <f>D6</f>
+        <v>5.9113618185921677</v>
+      </c>
+      <c r="K3" s="1">
+        <f>D12</f>
+        <v>6.2038836475592154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>0.2</v>
       </c>
@@ -1286,8 +3251,16 @@
       <c r="I4" s="1">
         <v>184</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="1">
+        <f>E6</f>
+        <v>5.5686309229805193</v>
+      </c>
+      <c r="K4" s="1">
+        <f>E12</f>
+        <v>6.1202964439509504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>0.17499999999999999</v>
       </c>
@@ -1322,16 +3295,60 @@
         <f t="shared" si="0"/>
         <v>169.66666666666666</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="1">
+        <f>F6</f>
+        <v>5.4260000479346377</v>
+      </c>
+      <c r="K5" s="1">
+        <f>F12</f>
+        <v>6.0014129279611508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>0.17499999999999999</v>
       </c>
       <c r="B6" s="2">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="1">
+        <f>(-0.405 * 0) + LN(C5)</f>
+        <v>5.6501472588235693</v>
+      </c>
+      <c r="D6" s="1">
+        <f>(-0.405 * A2) + LN(D5)</f>
+        <v>5.9113618185921677</v>
+      </c>
+      <c r="E6" s="1">
+        <f>(-0.405 * SUM(A2:A3)) + LN(E5)</f>
+        <v>5.5686309229805193</v>
+      </c>
+      <c r="F6" s="1">
+        <f>(-0.405 * SUM(A2:A4)) + LN(F5)</f>
+        <v>5.4260000479346377</v>
+      </c>
+      <c r="G6" s="1">
+        <f>(-0.405 * SUM(A2:A5)) + LN(G5)</f>
+        <v>5.2191456736714752</v>
+      </c>
+      <c r="H6" s="1">
+        <f>(-0.405 * SUM(A2:A7)) + LN(H5)</f>
+        <v>4.820060757608986</v>
+      </c>
+      <c r="I6" s="1">
+        <f>(-0.405 * SUM(A2:A9)) + LN(I5)</f>
+        <v>4.6369007278824137</v>
+      </c>
+      <c r="J6" s="1">
+        <f>G6</f>
+        <v>5.2191456736714752</v>
+      </c>
+      <c r="K6" s="1">
+        <f>G12</f>
+        <v>5.9089858877837438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>0.17499999999999999</v>
       </c>
@@ -1339,27 +3356,36 @@
         <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="1">
+        <f>H6</f>
+        <v>4.820060757608986</v>
+      </c>
+      <c r="K7" s="1">
+        <f>H12</f>
+        <v>5.8579302294834585</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
-        <v>0.13700000000000001</v>
+        <f>0.137 + 0.115</f>
+        <v>0.252</v>
       </c>
       <c r="B8" s="2">
         <v>127</v>
@@ -1382,11 +3408,12 @@
       <c r="H8" s="1">
         <v>380</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>0.115</v>
-      </c>
+      <c r="J8" s="1">
+        <f>I6</f>
+        <v>4.6369007278824137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="B9" s="2">
         <v>107</v>
       </c>
@@ -1409,10 +3436,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>0.15</v>
-      </c>
+    <row r="10" spans="1:11">
       <c r="B10" s="2">
         <v>131</v>
       </c>
@@ -1434,8 +3458,14 @@
       <c r="H10" s="1">
         <v>349</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="B11" s="2">
         <v>129</v>
       </c>
@@ -1463,1474 +3493,1523 @@
         <f t="shared" si="1"/>
         <v>350</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="1">
+        <f xml:space="preserve"> (C6 / D6) * 100</f>
+        <v>95.581144112224067</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
+        <f>(-A23 * A13) + LN(C11)</f>
+        <v>6.2105999795246527</v>
+      </c>
+      <c r="D12" s="1">
+        <f>(-A23 * A14) + LN(D11)</f>
+        <v>6.2038836475592154</v>
+      </c>
+      <c r="E12" s="1">
+        <f>(-A23 * A15) + LN(E11)</f>
+        <v>6.1202964439509504</v>
+      </c>
+      <c r="F12" s="1">
+        <f>(-A23 * A16) +LN(F11)</f>
+        <v>6.0014129279611508</v>
+      </c>
+      <c r="G12" s="1">
+        <f>(-A23 * A17) + LN(G11)</f>
+        <v>5.9089858877837438</v>
+      </c>
+      <c r="H12" s="1">
+        <f>(-A23 * A18) + LN(H11)</f>
+        <v>5.8579302294834585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
-        <v>1</v>
+        <f>1*1.3*10^-6</f>
+        <v>1.3E-6</v>
       </c>
       <c r="B13" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
-        <v>5</v>
+        <f>5 *1.3*10^-6</f>
+        <v>6.4999999999999996E-6</v>
       </c>
       <c r="B14" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
-        <v>10</v>
+        <f>10 *1.3*10^-6</f>
+        <v>1.2999999999999999E-5</v>
       </c>
       <c r="B15" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
-        <v>20</v>
+        <f xml:space="preserve"> 20 *(1.3*10^-6)</f>
+        <v>2.6000000000000002E-5</v>
       </c>
       <c r="B16" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>25</v>
+        <f>25*(1.3*10^-6)</f>
+        <v>3.2500000000000004E-5</v>
       </c>
       <c r="B17" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>30</v>
+        <f xml:space="preserve"> 30 * (1.3*10^-6)</f>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="B18" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="B19" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B20" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>0.40500000000000003</v>
+      </c>
       <c r="B21" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B22" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="B23" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="B24" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="B25" s="2">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="B26" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="B27" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="B28" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="B29" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="B30" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="B31" s="2">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="B32" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2">
       <c r="B33" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2">
       <c r="B34" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2">
       <c r="B35" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2">
       <c r="B36" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2">
       <c r="B37" s="2">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2">
       <c r="B38" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2">
       <c r="B39" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2">
       <c r="B40" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2">
       <c r="B41" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2">
       <c r="B42" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2">
       <c r="B43" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2">
       <c r="B44" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2">
       <c r="B45" s="2">
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2">
       <c r="B46" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2">
       <c r="B47" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2">
       <c r="B48" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2">
       <c r="B49" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2">
       <c r="B50" s="2">
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2">
       <c r="B51" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2">
       <c r="B52" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2">
       <c r="B53" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2">
       <c r="B54" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2">
       <c r="B55" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2">
       <c r="B56" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2">
       <c r="B57" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2">
       <c r="B58" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2">
       <c r="B59" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2">
       <c r="B60" s="2">
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2">
       <c r="B61" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2">
       <c r="B62" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2">
       <c r="B63" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2">
       <c r="B64" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2">
       <c r="B65" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2">
       <c r="B66" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2">
       <c r="B67" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2">
       <c r="B68" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2">
       <c r="B69" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2">
       <c r="B70" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2">
       <c r="B71" s="2">
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2">
       <c r="B72" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2">
       <c r="B73" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2">
       <c r="B74" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2">
       <c r="B75" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2">
       <c r="B76" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2">
       <c r="B77" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2">
       <c r="B78" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2">
       <c r="B79" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2">
       <c r="B80" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2">
       <c r="B81" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2">
       <c r="B82" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2">
       <c r="B83" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2">
       <c r="B84" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2">
       <c r="B85" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2">
       <c r="B86" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2">
       <c r="B87" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2">
       <c r="B88" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2">
       <c r="B89" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2">
       <c r="B90" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2">
       <c r="B91" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2">
       <c r="B92" s="2">
         <v>148</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2">
       <c r="B93" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2">
       <c r="B94" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2">
       <c r="B95" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2">
       <c r="B96" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2">
       <c r="B97" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2">
       <c r="B98" s="2">
         <v>144</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2">
       <c r="B99" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2">
       <c r="B100" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2">
       <c r="B101" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2">
       <c r="B102" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2">
       <c r="B103" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2">
       <c r="B104" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2">
       <c r="B105" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2">
       <c r="B106" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2">
       <c r="B107" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2">
       <c r="B108" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2">
       <c r="B109" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2">
       <c r="B110" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2">
       <c r="B111" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2">
       <c r="B112" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2">
       <c r="B113" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2">
       <c r="B114" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2">
       <c r="B115" s="2">
         <v>132</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2">
       <c r="B116" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2">
       <c r="B117" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2">
       <c r="B118" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2">
       <c r="B119" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2">
       <c r="B120" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2">
       <c r="B121" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2">
       <c r="B122" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2">
       <c r="B123" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2">
       <c r="B124" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2">
       <c r="B125" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2">
       <c r="B126" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2">
       <c r="B127" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2">
       <c r="B128" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2">
       <c r="B129" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2">
       <c r="B130" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2">
       <c r="B131" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2">
       <c r="B132" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2">
       <c r="B133" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2">
       <c r="B134" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2">
       <c r="B135" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2">
       <c r="B136" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2">
       <c r="B137" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2">
       <c r="B138" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2">
       <c r="B139" s="2">
         <v>113</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2">
       <c r="B140" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2">
       <c r="B141" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2">
       <c r="B142" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2">
       <c r="B143" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2">
       <c r="B144" s="2">
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2">
       <c r="B145" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2">
       <c r="B146" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2">
       <c r="B147" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2">
       <c r="B148" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2">
       <c r="B149" s="2">
         <v>144</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2">
       <c r="B150" s="2">
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2">
       <c r="B151" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2">
       <c r="B152" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2">
       <c r="B153" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2">
       <c r="B154" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2">
       <c r="B155" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2">
       <c r="B156" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2">
       <c r="B157" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2">
       <c r="B158" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2">
       <c r="B159" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2">
       <c r="B160" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2">
       <c r="B161" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2">
       <c r="B162" s="2">
         <v>112</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2">
       <c r="B163" s="2">
         <v>141</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2">
       <c r="B164" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2">
       <c r="B165" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2">
       <c r="B166" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2">
       <c r="B167" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2">
       <c r="B168" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2">
       <c r="B169" s="2">
         <v>126</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2">
       <c r="B170" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2">
       <c r="B171" s="2">
         <v>155</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2">
       <c r="B172" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2">
       <c r="B173" s="2">
         <v>141</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2">
       <c r="B174" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2">
       <c r="B175" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2">
       <c r="B176" s="2">
         <v>114</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2">
       <c r="B177" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2">
       <c r="B178" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2">
       <c r="B179" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2">
       <c r="B180" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2">
       <c r="B181" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2">
       <c r="B182" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2">
       <c r="B183" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2">
       <c r="B184" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2">
       <c r="B185" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2">
       <c r="B186" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2">
       <c r="B187" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2">
       <c r="B188" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2">
       <c r="B189" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2">
       <c r="B190" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2">
       <c r="B191" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2">
       <c r="B192" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2">
       <c r="B193" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2">
       <c r="B194" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2">
       <c r="B195" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2">
       <c r="B196" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2">
       <c r="B197" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2">
       <c r="B198" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2">
       <c r="B199" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2">
       <c r="B200" s="2">
         <v>132</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2">
       <c r="B201" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:2">
       <c r="B202" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:2">
       <c r="B203" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:2">
       <c r="B204" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:2">
       <c r="B205" s="2">
         <v>132</v>
       </c>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:2">
       <c r="B206" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:2">
       <c r="B207" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:2">
       <c r="B208" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:2">
       <c r="B209" s="2">
         <v>147</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:2">
       <c r="B210" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:2">
       <c r="B211" s="2">
         <v>94</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:2">
       <c r="B212" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:2">
       <c r="B213" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:2">
       <c r="B214" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:2">
       <c r="B215" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:2">
       <c r="B216" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:2">
       <c r="B217" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:2">
       <c r="B218" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:2">
       <c r="B219" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:2">
       <c r="B220" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:2">
       <c r="B221" s="2">
         <v>111</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:2">
       <c r="B222" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:2">
       <c r="B223" s="2">
         <v>132</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:2">
       <c r="B224" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:2">
       <c r="B225" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:2">
       <c r="B226" s="2">
         <v>148</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:2">
       <c r="B227" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:2">
       <c r="B228" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:2">
       <c r="B229" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:2">
       <c r="B230" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:2">
       <c r="B231" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:2">
       <c r="B232" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:2">
       <c r="B233" s="2">
         <v>118</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:2">
       <c r="B234" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:2">
       <c r="B235" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:2">
       <c r="B236" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:2">
       <c r="B237" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:2">
       <c r="B238" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:2">
       <c r="B239" s="2">
         <v>119</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:2">
       <c r="B240" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:2">
       <c r="B241" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:2">
       <c r="B242" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:2">
       <c r="B243" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:2">
       <c r="B244" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:2">
       <c r="B245" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:2">
       <c r="B246" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:2">
       <c r="B247" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:2">
       <c r="B248" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:2">
       <c r="B249" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:2">
       <c r="B250" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:2">
       <c r="B251" s="2">
         <v>147</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:2">
       <c r="B252" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:2">
       <c r="B253" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:2">
       <c r="B254" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:2">
       <c r="B255" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:2">
       <c r="B256" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:2">
       <c r="B257" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:2">
       <c r="B258" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:2">
       <c r="B259" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:2">
       <c r="B260" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:2">
       <c r="B261" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:2">
       <c r="B262" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:2">
       <c r="B263" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:2">
       <c r="B264" s="2">
         <v>141</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:2">
       <c r="B265" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:2">
       <c r="B266" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:2">
       <c r="B267" s="2">
         <v>117</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:2">
       <c r="B268" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:2">
       <c r="B269" s="2">
         <v>127</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:2">
       <c r="B270" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:2">
       <c r="B271" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:2">
       <c r="B272" s="2">
         <v>145</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:2">
       <c r="B273" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:2">
       <c r="B274" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:2">
       <c r="B275" s="2">
         <v>159</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:2">
       <c r="B276" s="2">
         <v>145</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:2">
       <c r="B277" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:2">
       <c r="B278" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:2">
       <c r="B279" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:2">
       <c r="B280" s="2">
         <v>116</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:2">
       <c r="B281" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:2">
       <c r="B282" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:2">
       <c r="B283" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:2">
       <c r="B284" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:2">
       <c r="B285" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:2">
       <c r="B286" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:2">
       <c r="B287" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:2">
       <c r="B288" s="2">
         <v>115</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:2">
       <c r="B289" s="2">
         <v>151</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:2">
       <c r="B290" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:2">
       <c r="B291" s="2">
         <v>155</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:2">
       <c r="B292" s="2">
         <v>122</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:2">
       <c r="B293" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:2">
       <c r="B294" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:2">
       <c r="B295" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:2">
       <c r="B296" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:2">
       <c r="B297" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:2">
       <c r="B298" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:2">
       <c r="B299" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:2">
       <c r="B300" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:2">
       <c r="B301" s="2">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
Adde content to report
</commit_message>
<xml_diff>
--- a/PS-250/Radioactivity_Lab/LabData.xlsx
+++ b/PS-250/Radioactivity_Lab/LabData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stark/StarkDev/Fall_2018_Homework/PS-250/Radioactivity_Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevStark\Github\Fall_2018_Homework\PS-250\Radioactivity_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9638356-EE29-904E-A875-7B6E2FCA583D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63907E38-2153-4FE5-A94E-FF1DA070C257}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15420" windowHeight="18000" xr2:uid="{1A1AC8B1-93FF-4B55-B881-409B33EC84FE}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="15420" windowHeight="18000" xr2:uid="{1A1AC8B1-93FF-4B55-B881-409B33EC84FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$301</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$301</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,14 +97,14 @@
     <t>Blocking Effectiveness % Al</t>
   </si>
   <si>
-    <t>=</t>
+    <t>Run #14 - Pb plate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +116,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Roboto Light"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,12 +138,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -207,7 +195,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>ln(N)</a:t>
+              <a:t>ln(N')</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -376,6 +364,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Plate Thicknes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -438,6 +481,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Readings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -559,7 +657,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>ln(N)</a:t>
+              <a:t>ln(N')</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -722,6 +820,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Foil</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Thickness</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -784,6 +942,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Readings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -833,37 +1046,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -963,10 +1145,66 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Number of Decays per reading</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Number of Decays per reading</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Recourence</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Recourence</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -2689,8 +2927,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3352800" y="3662362"/>
-              <a:ext cx="5184775" cy="2552700"/>
+              <a:off x="3146425" y="3948112"/>
+              <a:ext cx="4597400" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3094,27 +3332,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908E722D-64B1-4FB9-A7CE-2ED9FD62516E}">
   <dimension ref="A1:K301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="40.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3149,11 +3387,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.15</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>124</v>
       </c>
       <c r="C2" s="1">
@@ -3186,11 +3424,11 @@
         <v>6.2105999795246527</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>128</v>
       </c>
       <c r="C3" s="1">
@@ -3223,11 +3461,11 @@
         <v>6.2038836475592154</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>135</v>
       </c>
       <c r="C4" s="1">
@@ -3260,11 +3498,11 @@
         <v>6.1202964439509504</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.17499999999999999</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>118</v>
       </c>
       <c r="C5" s="1">
@@ -3304,11 +3542,11 @@
         <v>6.0014129279611508</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.17499999999999999</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>126</v>
       </c>
       <c r="C6" s="1">
@@ -3348,11 +3586,11 @@
         <v>5.9089858877837438</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.17499999999999999</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -3372,6 +3610,9 @@
       </c>
       <c r="H7" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J7" s="1">
         <f>H6</f>
@@ -3382,12 +3623,12 @@
         <v>5.8579302294834585</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>0.137 + 0.115</f>
         <v>0.252</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>127</v>
       </c>
       <c r="C8" s="1">
@@ -3407,14 +3648,17 @@
       </c>
       <c r="H8" s="1">
         <v>380</v>
+      </c>
+      <c r="I8" s="1">
+        <v>25</v>
       </c>
       <c r="J8" s="1">
         <f>I6</f>
         <v>4.6369007278824137</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="B9" s="2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
         <v>107</v>
       </c>
       <c r="C9" s="1">
@@ -3435,9 +3679,12 @@
       <c r="H9" s="1">
         <v>321</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="B10" s="2">
+      <c r="I9" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
         <v>131</v>
       </c>
       <c r="C10" s="1">
@@ -3458,6 +3705,9 @@
       <c r="H10" s="1">
         <v>349</v>
       </c>
+      <c r="I10" s="1">
+        <v>34</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>20</v>
       </c>
@@ -3465,8 +3715,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
         <v>129</v>
       </c>
       <c r="C11" s="1">
@@ -3493,19 +3743,24 @@
         <f t="shared" si="1"/>
         <v>350</v>
       </c>
+      <c r="I11" s="1">
+        <f>AVERAGE(I8:I10)</f>
+        <v>27.666666666666668</v>
+      </c>
       <c r="J11" s="1">
         <f xml:space="preserve"> (C6 / D6) * 100</f>
         <v>95.581144112224067</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="K11" s="1">
+        <f xml:space="preserve"> (I11 / C11) * 100</f>
+        <v>5.5555555555555562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>128</v>
       </c>
       <c r="C12" s="1">
@@ -3533,1484 +3788,1484 @@
         <v>5.8579302294834585</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>1*1.3*10^-6</f>
         <v>1.3E-6</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>5 *1.3*10^-6</f>
         <v>6.4999999999999996E-6</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f>10 *1.3*10^-6</f>
         <v>1.2999999999999999E-5</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f xml:space="preserve"> 20 *(1.3*10^-6)</f>
         <v>2.6000000000000002E-5</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f>25*(1.3*10^-6)</f>
         <v>3.2500000000000004E-5</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f xml:space="preserve"> 30 * (1.3*10^-6)</f>
         <v>3.8999999999999999E-5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="B19" s="2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.40500000000000003</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="B24" s="2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="B25" s="2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="B26" s="2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="B27" s="2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="B28" s="2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="B29" s="2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="B30" s="2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="B31" s="2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="B32" s="2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1">
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
-      <c r="B66" s="2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="2:2">
-      <c r="B69" s="2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="2:2">
-      <c r="B70" s="2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
-      <c r="B71" s="2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1">
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="2:2">
-      <c r="B72" s="2">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="2:2">
-      <c r="B73" s="2">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2">
-      <c r="B74" s="2">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="2:2">
-      <c r="B75" s="2">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="76" spans="2:2">
-      <c r="B76" s="2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="2:2">
-      <c r="B77" s="2">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="2:2">
-      <c r="B78" s="2">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="2:2">
-      <c r="B79" s="2">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="2:2">
-      <c r="B80" s="2">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="2:2">
-      <c r="B82" s="2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="2:2">
-      <c r="B83" s="2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="2:2">
-      <c r="B84" s="2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="2:2">
-      <c r="B85" s="2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
-      <c r="B86" s="2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
-      <c r="B87" s="2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="88" spans="2:2">
-      <c r="B88" s="2">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="89" spans="2:2">
-      <c r="B89" s="2">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="2:2">
-      <c r="B90" s="2">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="2:2">
-      <c r="B91" s="2">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="92" spans="2:2">
-      <c r="B92" s="2">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1">
         <v>148</v>
       </c>
     </row>
-    <row r="93" spans="2:2">
-      <c r="B93" s="2">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="2:2">
-      <c r="B94" s="2">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="2:2">
-      <c r="B95" s="2">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2">
-      <c r="B96" s="2">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="2:2">
-      <c r="B97" s="2">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="2:2">
-      <c r="B98" s="2">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1">
         <v>144</v>
       </c>
     </row>
-    <row r="99" spans="2:2">
-      <c r="B99" s="2">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="2:2">
-      <c r="B100" s="2">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="2:2">
-      <c r="B101" s="2">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="2:2">
-      <c r="B102" s="2">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="2:2">
-      <c r="B103" s="2">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="2:2">
-      <c r="B104" s="2">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="2:2">
-      <c r="B105" s="2">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="2:2">
-      <c r="B106" s="2">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="107" spans="2:2">
-      <c r="B107" s="2">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="2:2">
-      <c r="B108" s="2">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="1">
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="2:2">
-      <c r="B109" s="2">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="2:2">
-      <c r="B110" s="2">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="2:2">
-      <c r="B111" s="2">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="2:2">
-      <c r="B112" s="2">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="2:2">
-      <c r="B113" s="2">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="114" spans="2:2">
-      <c r="B114" s="2">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="2:2">
-      <c r="B115" s="2">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="1">
         <v>132</v>
       </c>
     </row>
-    <row r="116" spans="2:2">
-      <c r="B116" s="2">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="2:2">
-      <c r="B117" s="2">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="118" spans="2:2">
-      <c r="B118" s="2">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="119" spans="2:2">
-      <c r="B119" s="2">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="120" spans="2:2">
-      <c r="B120" s="2">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="2:2">
-      <c r="B121" s="2">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="2:2">
-      <c r="B122" s="2">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="2:2">
-      <c r="B123" s="2">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="2:2">
-      <c r="B124" s="2">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="2:2">
-      <c r="B125" s="2">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="2:2">
-      <c r="B126" s="2">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="2:2">
-      <c r="B127" s="2">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="128" spans="2:2">
-      <c r="B128" s="2">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="2:2">
-      <c r="B129" s="2">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="2:2">
-      <c r="B130" s="2">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="131" spans="2:2">
-      <c r="B131" s="2">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="132" spans="2:2">
-      <c r="B132" s="2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="133" spans="2:2">
-      <c r="B133" s="2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="2:2">
-      <c r="B134" s="2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="135" spans="2:2">
-      <c r="B135" s="2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="136" spans="2:2">
-      <c r="B136" s="2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="137" spans="2:2">
-      <c r="B137" s="2">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="138" spans="2:2">
-      <c r="B138" s="2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="139" spans="2:2">
-      <c r="B139" s="2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" s="1">
         <v>113</v>
       </c>
     </row>
-    <row r="140" spans="2:2">
-      <c r="B140" s="2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="141" spans="2:2">
-      <c r="B141" s="2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="142" spans="2:2">
-      <c r="B142" s="2">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="143" spans="2:2">
-      <c r="B143" s="2">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="144" spans="2:2">
-      <c r="B144" s="2">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B144" s="1">
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
-      <c r="B145" s="2">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="146" spans="2:2">
-      <c r="B146" s="2">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="147" spans="2:2">
-      <c r="B147" s="2">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="148" spans="2:2">
-      <c r="B148" s="2">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="149" spans="2:2">
-      <c r="B149" s="2">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B149" s="1">
         <v>144</v>
       </c>
     </row>
-    <row r="150" spans="2:2">
-      <c r="B150" s="2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="1">
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="2:2">
-      <c r="B151" s="2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="152" spans="2:2">
-      <c r="B152" s="2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B152" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="153" spans="2:2">
-      <c r="B153" s="2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="154" spans="2:2">
-      <c r="B154" s="2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="155" spans="2:2">
-      <c r="B155" s="2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="2:2">
-      <c r="B156" s="2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="157" spans="2:2">
-      <c r="B157" s="2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="158" spans="2:2">
-      <c r="B158" s="2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="1">
         <v>136</v>
       </c>
     </row>
-    <row r="159" spans="2:2">
-      <c r="B159" s="2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="160" spans="2:2">
-      <c r="B160" s="2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="161" spans="2:2">
-      <c r="B161" s="2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="2:2">
-      <c r="B162" s="2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="163" spans="2:2">
-      <c r="B163" s="2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="1">
         <v>141</v>
       </c>
     </row>
-    <row r="164" spans="2:2">
-      <c r="B164" s="2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B164" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="165" spans="2:2">
-      <c r="B165" s="2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="166" spans="2:2">
-      <c r="B166" s="2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B166" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="167" spans="2:2">
-      <c r="B167" s="2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="168" spans="2:2">
-      <c r="B168" s="2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="169" spans="2:2">
-      <c r="B169" s="2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B169" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="170" spans="2:2">
-      <c r="B170" s="2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="171" spans="2:2">
-      <c r="B171" s="2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B171" s="1">
         <v>155</v>
       </c>
     </row>
-    <row r="172" spans="2:2">
-      <c r="B172" s="2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B172" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="173" spans="2:2">
-      <c r="B173" s="2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B173" s="1">
         <v>141</v>
       </c>
     </row>
-    <row r="174" spans="2:2">
-      <c r="B174" s="2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="175" spans="2:2">
-      <c r="B175" s="2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B175" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="176" spans="2:2">
-      <c r="B176" s="2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B176" s="1">
         <v>114</v>
       </c>
     </row>
-    <row r="177" spans="2:2">
-      <c r="B177" s="2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B177" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="178" spans="2:2">
-      <c r="B178" s="2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B178" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="179" spans="2:2">
-      <c r="B179" s="2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B179" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="2:2">
-      <c r="B180" s="2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B180" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="181" spans="2:2">
-      <c r="B181" s="2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B181" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="182" spans="2:2">
-      <c r="B182" s="2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B182" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="183" spans="2:2">
-      <c r="B183" s="2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B183" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="184" spans="2:2">
-      <c r="B184" s="2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B184" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="185" spans="2:2">
-      <c r="B185" s="2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B185" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="186" spans="2:2">
-      <c r="B186" s="2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B186" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="187" spans="2:2">
-      <c r="B187" s="2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B187" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="188" spans="2:2">
-      <c r="B188" s="2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B188" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="189" spans="2:2">
-      <c r="B189" s="2">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B189" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="190" spans="2:2">
-      <c r="B190" s="2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B190" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="191" spans="2:2">
-      <c r="B191" s="2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B191" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="192" spans="2:2">
-      <c r="B192" s="2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B192" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="193" spans="2:2">
-      <c r="B193" s="2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B193" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="194" spans="2:2">
-      <c r="B194" s="2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B194" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="195" spans="2:2">
-      <c r="B195" s="2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B195" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="196" spans="2:2">
-      <c r="B196" s="2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B196" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="197" spans="2:2">
-      <c r="B197" s="2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B197" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="198" spans="2:2">
-      <c r="B198" s="2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B198" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="199" spans="2:2">
-      <c r="B199" s="2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="200" spans="2:2">
-      <c r="B200" s="2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B200" s="1">
         <v>132</v>
       </c>
     </row>
-    <row r="201" spans="2:2">
-      <c r="B201" s="2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="202" spans="2:2">
-      <c r="B202" s="2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B202" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="203" spans="2:2">
-      <c r="B203" s="2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B203" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="204" spans="2:2">
-      <c r="B204" s="2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B204" s="1">
         <v>136</v>
       </c>
     </row>
-    <row r="205" spans="2:2">
-      <c r="B205" s="2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B205" s="1">
         <v>132</v>
       </c>
     </row>
-    <row r="206" spans="2:2">
-      <c r="B206" s="2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B206" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="207" spans="2:2">
-      <c r="B207" s="2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B207" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="208" spans="2:2">
-      <c r="B208" s="2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B208" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="209" spans="2:2">
-      <c r="B209" s="2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B209" s="1">
         <v>147</v>
       </c>
     </row>
-    <row r="210" spans="2:2">
-      <c r="B210" s="2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B210" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="211" spans="2:2">
-      <c r="B211" s="2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B211" s="1">
         <v>94</v>
       </c>
     </row>
-    <row r="212" spans="2:2">
-      <c r="B212" s="2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B212" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="213" spans="2:2">
-      <c r="B213" s="2">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B213" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="214" spans="2:2">
-      <c r="B214" s="2">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B214" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="215" spans="2:2">
-      <c r="B215" s="2">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B215" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="216" spans="2:2">
-      <c r="B216" s="2">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B216" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="217" spans="2:2">
-      <c r="B217" s="2">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B217" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="218" spans="2:2">
-      <c r="B218" s="2">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B218" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="219" spans="2:2">
-      <c r="B219" s="2">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B219" s="1">
         <v>136</v>
       </c>
     </row>
-    <row r="220" spans="2:2">
-      <c r="B220" s="2">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B220" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="221" spans="2:2">
-      <c r="B221" s="2">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B221" s="1">
         <v>111</v>
       </c>
     </row>
-    <row r="222" spans="2:2">
-      <c r="B222" s="2">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B222" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="223" spans="2:2">
-      <c r="B223" s="2">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B223" s="1">
         <v>132</v>
       </c>
     </row>
-    <row r="224" spans="2:2">
-      <c r="B224" s="2">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B224" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="225" spans="2:2">
-      <c r="B225" s="2">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B225" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="226" spans="2:2">
-      <c r="B226" s="2">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B226" s="1">
         <v>148</v>
       </c>
     </row>
-    <row r="227" spans="2:2">
-      <c r="B227" s="2">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B227" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="228" spans="2:2">
-      <c r="B228" s="2">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B228" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="229" spans="2:2">
-      <c r="B229" s="2">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B229" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="230" spans="2:2">
-      <c r="B230" s="2">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B230" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="231" spans="2:2">
-      <c r="B231" s="2">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B231" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="232" spans="2:2">
-      <c r="B232" s="2">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B232" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="233" spans="2:2">
-      <c r="B233" s="2">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B233" s="1">
         <v>118</v>
       </c>
     </row>
-    <row r="234" spans="2:2">
-      <c r="B234" s="2">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B234" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="235" spans="2:2">
-      <c r="B235" s="2">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B235" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="236" spans="2:2">
-      <c r="B236" s="2">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B236" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="237" spans="2:2">
-      <c r="B237" s="2">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B237" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="238" spans="2:2">
-      <c r="B238" s="2">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B238" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="239" spans="2:2">
-      <c r="B239" s="2">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B239" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="240" spans="2:2">
-      <c r="B240" s="2">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B240" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="241" spans="2:2">
-      <c r="B241" s="2">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B241" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="242" spans="2:2">
-      <c r="B242" s="2">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B242" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="243" spans="2:2">
-      <c r="B243" s="2">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B243" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="244" spans="2:2">
-      <c r="B244" s="2">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B244" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="245" spans="2:2">
-      <c r="B245" s="2">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B245" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="246" spans="2:2">
-      <c r="B246" s="2">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B246" s="1">
         <v>138</v>
       </c>
     </row>
-    <row r="247" spans="2:2">
-      <c r="B247" s="2">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B247" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="248" spans="2:2">
-      <c r="B248" s="2">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B248" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="249" spans="2:2">
-      <c r="B249" s="2">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B249" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="250" spans="2:2">
-      <c r="B250" s="2">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B250" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="251" spans="2:2">
-      <c r="B251" s="2">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B251" s="1">
         <v>147</v>
       </c>
     </row>
-    <row r="252" spans="2:2">
-      <c r="B252" s="2">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B252" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="253" spans="2:2">
-      <c r="B253" s="2">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B253" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="254" spans="2:2">
-      <c r="B254" s="2">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B254" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="255" spans="2:2">
-      <c r="B255" s="2">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B255" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="256" spans="2:2">
-      <c r="B256" s="2">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B256" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="257" spans="2:2">
-      <c r="B257" s="2">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B257" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="258" spans="2:2">
-      <c r="B258" s="2">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B258" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="259" spans="2:2">
-      <c r="B259" s="2">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B259" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="260" spans="2:2">
-      <c r="B260" s="2">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B260" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="261" spans="2:2">
-      <c r="B261" s="2">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B261" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="262" spans="2:2">
-      <c r="B262" s="2">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B262" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="263" spans="2:2">
-      <c r="B263" s="2">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B263" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="264" spans="2:2">
-      <c r="B264" s="2">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B264" s="1">
         <v>141</v>
       </c>
     </row>
-    <row r="265" spans="2:2">
-      <c r="B265" s="2">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B265" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="266" spans="2:2">
-      <c r="B266" s="2">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B266" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="267" spans="2:2">
-      <c r="B267" s="2">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B267" s="1">
         <v>117</v>
       </c>
     </row>
-    <row r="268" spans="2:2">
-      <c r="B268" s="2">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B268" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="269" spans="2:2">
-      <c r="B269" s="2">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B269" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="270" spans="2:2">
-      <c r="B270" s="2">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B270" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="271" spans="2:2">
-      <c r="B271" s="2">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B271" s="1">
         <v>137</v>
       </c>
     </row>
-    <row r="272" spans="2:2">
-      <c r="B272" s="2">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B272" s="1">
         <v>145</v>
       </c>
     </row>
-    <row r="273" spans="2:2">
-      <c r="B273" s="2">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B273" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="274" spans="2:2">
-      <c r="B274" s="2">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B274" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="275" spans="2:2">
-      <c r="B275" s="2">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B275" s="1">
         <v>159</v>
       </c>
     </row>
-    <row r="276" spans="2:2">
-      <c r="B276" s="2">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B276" s="1">
         <v>145</v>
       </c>
     </row>
-    <row r="277" spans="2:2">
-      <c r="B277" s="2">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B277" s="1">
         <v>130</v>
       </c>
     </row>
-    <row r="278" spans="2:2">
-      <c r="B278" s="2">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B278" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="279" spans="2:2">
-      <c r="B279" s="2">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B279" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="280" spans="2:2">
-      <c r="B280" s="2">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B280" s="1">
         <v>116</v>
       </c>
     </row>
-    <row r="281" spans="2:2">
-      <c r="B281" s="2">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B281" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="282" spans="2:2">
-      <c r="B282" s="2">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B282" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="283" spans="2:2">
-      <c r="B283" s="2">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B283" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="284" spans="2:2">
-      <c r="B284" s="2">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B284" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="285" spans="2:2">
-      <c r="B285" s="2">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B285" s="1">
         <v>134</v>
       </c>
     </row>
-    <row r="286" spans="2:2">
-      <c r="B286" s="2">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B286" s="1">
         <v>128</v>
       </c>
     </row>
-    <row r="287" spans="2:2">
-      <c r="B287" s="2">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B287" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="288" spans="2:2">
-      <c r="B288" s="2">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B288" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="289" spans="2:2">
-      <c r="B289" s="2">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B289" s="1">
         <v>151</v>
       </c>
     </row>
-    <row r="290" spans="2:2">
-      <c r="B290" s="2">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B290" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="291" spans="2:2">
-      <c r="B291" s="2">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B291" s="1">
         <v>155</v>
       </c>
     </row>
-    <row r="292" spans="2:2">
-      <c r="B292" s="2">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B292" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="293" spans="2:2">
-      <c r="B293" s="2">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B293" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="294" spans="2:2">
-      <c r="B294" s="2">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B294" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="295" spans="2:2">
-      <c r="B295" s="2">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B295" s="1">
         <v>133</v>
       </c>
     </row>
-    <row r="296" spans="2:2">
-      <c r="B296" s="2">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B296" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="297" spans="2:2">
-      <c r="B297" s="2">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B297" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="298" spans="2:2">
-      <c r="B298" s="2">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B298" s="1">
         <v>139</v>
       </c>
     </row>
-    <row r="299" spans="2:2">
-      <c r="B299" s="2">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B299" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="300" spans="2:2">
-      <c r="B300" s="2">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B300" s="1">
         <v>129</v>
       </c>
     </row>
-    <row r="301" spans="2:2">
-      <c r="B301" s="2">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B301" s="1">
         <v>142</v>
       </c>
     </row>

</xml_diff>